<commit_message>
Nombres a mapa Choco
</commit_message>
<xml_diff>
--- a/data/Data_Choco.xlsx
+++ b/data/Data_Choco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Eli PAHO\Otros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Eli PAHO\GIT\maps-\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -578,7 +578,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -589,6 +589,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="8" builtinId="30" customBuiltin="1"/>
@@ -911,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D2" sqref="D2:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +953,7 @@
       <c r="C2" s="1">
         <v>27001</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1">
@@ -966,7 +970,7 @@
       <c r="C3" s="1">
         <v>27006</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -983,7 +987,7 @@
       <c r="C4" s="1">
         <v>27025</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="1">
@@ -1000,7 +1004,7 @@
       <c r="C5" s="1">
         <v>27050</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="1">
@@ -1017,7 +1021,7 @@
       <c r="C6" s="1">
         <v>27073</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="1">
@@ -1034,7 +1038,7 @@
       <c r="C7" s="1">
         <v>27075</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1">
@@ -1051,7 +1055,7 @@
       <c r="C8" s="1">
         <v>27077</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1">
@@ -1068,7 +1072,7 @@
       <c r="C9" s="1">
         <v>27099</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1">
@@ -1085,7 +1089,7 @@
       <c r="C10" s="1">
         <v>27135</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1">
@@ -1102,7 +1106,7 @@
       <c r="C11" s="1">
         <v>27150</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1">
@@ -1119,7 +1123,7 @@
       <c r="C12" s="1">
         <v>27160</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1">
@@ -1136,7 +1140,7 @@
       <c r="C13" s="1">
         <v>27205</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1">
@@ -1153,7 +1157,7 @@
       <c r="C14" s="1">
         <v>27245</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="1">
@@ -1170,7 +1174,7 @@
       <c r="C15" s="1">
         <v>27250</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1">
@@ -1187,7 +1191,7 @@
       <c r="C16" s="1">
         <v>27361</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="1">
@@ -1204,7 +1208,7 @@
       <c r="C17" s="1">
         <v>27372</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="1">
@@ -1221,7 +1225,7 @@
       <c r="C18" s="1">
         <v>27413</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="1">
@@ -1238,7 +1242,7 @@
       <c r="C19" s="1">
         <v>27425</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="1">
@@ -1255,7 +1259,7 @@
       <c r="C20" s="1">
         <v>27430</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="1">
@@ -1272,7 +1276,7 @@
       <c r="C21" s="1">
         <v>27450</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="1">
@@ -1289,7 +1293,7 @@
       <c r="C22" s="1">
         <v>27491</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="1">
@@ -1306,7 +1310,7 @@
       <c r="C23" s="1">
         <v>27495</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="1">
@@ -1323,7 +1327,7 @@
       <c r="C24" s="1">
         <v>27580</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="1">
@@ -1340,7 +1344,7 @@
       <c r="C25" s="1">
         <v>27600</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="1">
@@ -1357,7 +1361,7 @@
       <c r="C26" s="1">
         <v>27615</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="1">
@@ -1374,7 +1378,7 @@
       <c r="C27" s="1">
         <v>27660</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="1">
@@ -1391,7 +1395,7 @@
       <c r="C28" s="1">
         <v>27745</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="1">
@@ -1408,7 +1412,7 @@
       <c r="C29" s="1">
         <v>27787</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="1">
@@ -1425,7 +1429,7 @@
       <c r="C30" s="1">
         <v>27800</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="1">
@@ -1442,12 +1446,15 @@
       <c r="C31" s="1">
         <v>27810</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E31" s="1">
         <v>6982</v>
       </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E31"/>

</xml_diff>